<commit_message>
reemplazando caldas por manizales
</commit_message>
<xml_diff>
--- a/ciudades.xlsx
+++ b/ciudades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Cod Mun</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Tulua</t>
+  </si>
+  <si>
+    <t>Manizales</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -605,22 +608,22 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>5129</v>
+        <v>17001</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="E8" s="3">
-        <v>6.0909950000000004</v>
+        <v>5.07</v>
       </c>
       <c r="F8">
-        <v>-75.635568000000006</v>
+        <v>-75.520555599999994</v>
       </c>
     </row>
     <row r="9" spans="1:6">

</xml_diff>